<commit_message>
All flash spreadsheet mods
</commit_message>
<xml_diff>
--- a/assets/all-flash-calculator.xlsx
+++ b/assets/all-flash-calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken/repos/aerospike-ansible/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32AD55A-3E34-5F46-986F-696D4466FBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22EA900-AD5A-8F4F-9DDC-30AE747EF23E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{071011FB-609B-454D-B77B-CC151657AF81}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>Rounded Sprigs per partition</t>
   </si>
   <si>
-    <t>Overhead per per record</t>
-  </si>
-  <si>
     <t>Free disk pct</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Partitions Per Device</t>
+  </si>
+  <si>
+    <t>Overhead per per record (bytes)</t>
   </si>
 </sst>
 </file>
@@ -608,13 +608,13 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="19" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.83203125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5" style="14" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="9" customWidth="1"/>
@@ -646,7 +646,7 @@
         <v>4096</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>4096</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5">
         <f>C5*C11*C4*C3/1024^3</f>
@@ -755,7 +755,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="12" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C15" s="5">
         <f>CEILING(C13 * 1024^3/(C2 * 10^6)/C4,1)</f>
@@ -771,7 +771,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4">
         <v>0.5</v>
@@ -786,7 +786,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1">
         <v>1024</v>
@@ -796,7 +796,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="5">
         <f>AllFlashOverheadPerRecord+C19</f>
@@ -807,7 +807,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="5">
         <f>C20+C19</f>
@@ -823,7 +823,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="7">
         <f>C21*C2*10^6/10^12</f>
@@ -839,7 +839,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="7">
         <f>CEILING(C21/AllFlashOverheadPerRecord,1)</f>

</xml_diff>